<commit_message>
added sliders and did graph work
</commit_message>
<xml_diff>
--- a/FilmFinder/FilmFinder/bin/Release/Subject 1 - Hina.xlsx
+++ b/FilmFinder/FilmFinder/bin/Release/Subject 1 - Hina.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="15">
   <si>
     <t>Actor</t>
   </si>
@@ -41,9 +41,6 @@
     <t>active</t>
   </si>
   <si>
-    <t>mosuewheel</t>
-  </si>
-  <si>
     <t>list1</t>
   </si>
   <si>
@@ -51,6 +48,18 @@
   </si>
   <si>
     <t>mousewheel</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>list</t>
   </si>
 </sst>
 </file>
@@ -638,10 +647,10 @@
                   <c:v>active</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>mosuewheel</c:v>
+                  <c:v>mousewheel</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>list1</c:v>
+                  <c:v>list</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -686,11 +695,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="99534336"/>
-        <c:axId val="99535872"/>
+        <c:axId val="79291136"/>
+        <c:axId val="79293056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="99534336"/>
+        <c:axId val="79291136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -699,7 +708,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99535872"/>
+        <c:crossAx val="79293056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -707,7 +716,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99535872"/>
+        <c:axId val="79293056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -718,11 +727,16 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99534336"/>
+        <c:crossAx val="79291136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -761,7 +775,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Subject 1'!$J$6</c:f>
+              <c:f>'Subject 1'!$J$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -773,7 +787,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Subject 1'!$I$7:$I$13</c:f>
+              <c:f>'Subject 1'!$I$20:$I$26</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -792,17 +806,17 @@
                   <c:v>active</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>mosuewheel</c:v>
+                  <c:v>mousewheel</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>list1</c:v>
+                  <c:v>list</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Subject 1'!$J$7:$J$13</c:f>
+              <c:f>'Subject 1'!$J$20:$J$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -836,7 +850,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Subject 1'!$K$6</c:f>
+              <c:f>'Subject 1'!$K$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -848,7 +862,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Subject 1'!$I$7:$I$13</c:f>
+              <c:f>'Subject 1'!$I$20:$I$26</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -867,17 +881,17 @@
                   <c:v>active</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>mosuewheel</c:v>
+                  <c:v>mousewheel</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>list1</c:v>
+                  <c:v>list</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Subject 1'!$K$7:$K$13</c:f>
+              <c:f>'Subject 1'!$K$20:$K$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -911,7 +925,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Subject 1'!$L$6</c:f>
+              <c:f>'Subject 1'!$L$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -923,7 +937,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Subject 1'!$I$7:$I$13</c:f>
+              <c:f>'Subject 1'!$I$20:$I$26</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -942,17 +956,17 @@
                   <c:v>active</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>mosuewheel</c:v>
+                  <c:v>mousewheel</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>list1</c:v>
+                  <c:v>list</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Subject 1'!$L$7:$L$13</c:f>
+              <c:f>'Subject 1'!$L$20:$L$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -990,11 +1004,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="100360192"/>
-        <c:axId val="100361728"/>
+        <c:axId val="43241856"/>
+        <c:axId val="43243392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="100360192"/>
+        <c:axId val="43241856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1003,7 +1017,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100361728"/>
+        <c:crossAx val="43243392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1011,7 +1025,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100361728"/>
+        <c:axId val="43243392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1022,7 +1036,316 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100360192"/>
+        <c:crossAx val="43241856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Subject 1'!$I$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Low</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Subject 1'!$J$35:$P$35</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>trackbar</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>alpha</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>multi</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>histo</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>active</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>mousewheel</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>list</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Subject 1'!$J$36:$P$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>11186</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26289.666666666668</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14318.666666666666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65200.333333333336</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22839.666666666668</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13711</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13101.333333333334</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Subject 1'!$I$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Medium</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Subject 1'!$J$35:$P$35</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>trackbar</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>alpha</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>multi</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>histo</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>active</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>mousewheel</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>list</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Subject 1'!$J$37:$P$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>16817</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22193.666666666668</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31269</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>114660.66666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22751</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24976</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43402.333333333336</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Subject 1'!$I$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>High</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Subject 1'!$J$35:$P$35</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>trackbar</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>alpha</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>multi</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>histo</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>active</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>mousewheel</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>list</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Subject 1'!$J$38:$P$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>14486</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17978</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39842</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45328.333333333336</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18057.666666666668</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28124.333333333332</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13643.666666666666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="45409408"/>
+        <c:axId val="45411712"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="45409408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="45411712"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="45411712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="45409408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1049,19 +1372,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
+      <xdr:colOff>438150</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1078,20 +1401,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
+      <xdr:colOff>333375</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="6" name="Chart 5"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1101,6 +1424,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1396,10 +1749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N63"/>
+  <dimension ref="A1:P63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1439,10 +1792,10 @@
         <v>7</v>
       </c>
       <c r="M1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1473,23 +1826,23 @@
         <v>22153.777777777777</v>
       </c>
       <c r="J2">
+        <f>AVERAGE(E19:E27)</f>
+        <v>28476.555555555555</v>
+      </c>
+      <c r="K2">
         <f>AVERAGE(E28:E36)</f>
-        <v>28476.555555555555</v>
-      </c>
-      <c r="K2">
+        <v>75063.111111111109</v>
+      </c>
+      <c r="L2">
+        <f>AVERAGE(E37:E45)</f>
+        <v>21216.111111111109</v>
+      </c>
+      <c r="M2">
         <f>AVERAGE(E46:E54)</f>
-        <v>75063.111111111109</v>
-      </c>
-      <c r="L2">
+        <v>22270.444444444445</v>
+      </c>
+      <c r="N2">
         <f>AVERAGE(E55:E63)</f>
-        <v>21216.111111111109</v>
-      </c>
-      <c r="M2">
-        <f>AVERAGE(E37:E45)</f>
-        <v>22270.444444444445</v>
-      </c>
-      <c r="N2">
-        <f>AVERAGE(E19:E27)</f>
         <v>23382.444444444445</v>
       </c>
     </row>
@@ -1572,15 +1925,6 @@
       <c r="F6" t="b">
         <v>1</v>
       </c>
-      <c r="J6" t="s">
-        <v>0</v>
-      </c>
-      <c r="K6" t="s">
-        <v>1</v>
-      </c>
-      <c r="L6" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1601,21 +1945,6 @@
       <c r="F7" t="b">
         <v>1</v>
       </c>
-      <c r="I7" t="s">
-        <v>3</v>
-      </c>
-      <c r="J7">
-        <f>AVERAGE(E1:E3)</f>
-        <v>17951</v>
-      </c>
-      <c r="K7">
-        <f>AVERAGE(E4:E6)</f>
-        <v>10849</v>
-      </c>
-      <c r="L7">
-        <f>AVERAGE(E7:E9)</f>
-        <v>13689</v>
-      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1636,21 +1965,6 @@
       <c r="F8" t="b">
         <v>1</v>
       </c>
-      <c r="I8" t="s">
-        <v>4</v>
-      </c>
-      <c r="J8">
-        <f>AVERAGE(E10:E12)</f>
-        <v>25999</v>
-      </c>
-      <c r="K8">
-        <f>AVERAGE(E13:E15)</f>
-        <v>19660.666666666668</v>
-      </c>
-      <c r="L8">
-        <f>AVERAGE(E16:E18)</f>
-        <v>20801.666666666668</v>
-      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -1671,21 +1985,6 @@
       <c r="F9" t="b">
         <v>1</v>
       </c>
-      <c r="I9" t="s">
-        <v>5</v>
-      </c>
-      <c r="J9">
-        <f>AVERAGE(E28:E30)</f>
-        <v>42292</v>
-      </c>
-      <c r="K9">
-        <f>AVERAGE(E31:E33)</f>
-        <v>29080</v>
-      </c>
-      <c r="L9">
-        <f>AVERAGE(E34:E36)</f>
-        <v>14057.666666666666</v>
-      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1706,21 +2005,6 @@
       <c r="F10" t="b">
         <v>1</v>
       </c>
-      <c r="I10" t="s">
-        <v>6</v>
-      </c>
-      <c r="J10">
-        <f>AVERAGE(E46:E48)</f>
-        <v>135445.33333333334</v>
-      </c>
-      <c r="K10">
-        <f>AVERAGE(E49:E51)</f>
-        <v>53236.333333333336</v>
-      </c>
-      <c r="L10">
-        <f>AVERAGE(E52:E54)</f>
-        <v>36507.666666666664</v>
-      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1741,21 +2025,6 @@
       <c r="F11" t="b">
         <v>1</v>
       </c>
-      <c r="I11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J11">
-        <f>AVERAGE(E55:E57)</f>
-        <v>17131</v>
-      </c>
-      <c r="K11">
-        <f>AVERAGE(E58:E60)</f>
-        <v>31390.333333333332</v>
-      </c>
-      <c r="L11">
-        <f>AVERAGE(E61:E63)</f>
-        <v>15127</v>
-      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1776,21 +2045,6 @@
       <c r="F12" t="b">
         <v>1</v>
       </c>
-      <c r="I12" t="s">
-        <v>8</v>
-      </c>
-      <c r="J12">
-        <f>AVERAGE(E37:E39)</f>
-        <v>22500</v>
-      </c>
-      <c r="K12">
-        <f>AVERAGE(E40:E42)</f>
-        <v>32767</v>
-      </c>
-      <c r="L12">
-        <f>AVERAGE(E43:E45)</f>
-        <v>11544.333333333334</v>
-      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1811,21 +2065,6 @@
       <c r="F13" t="b">
         <v>1</v>
       </c>
-      <c r="I13" t="s">
-        <v>9</v>
-      </c>
-      <c r="J13">
-        <f>AVERAGE(E19:E21)</f>
-        <v>29840</v>
-      </c>
-      <c r="K13">
-        <f>AVERAGE(E22:E24)</f>
-        <v>27985.666666666668</v>
-      </c>
-      <c r="L13">
-        <f>AVERAGE(E25:E27)</f>
-        <v>12321.666666666666</v>
-      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1887,7 +2126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1907,7 +2146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1927,1132 +2166,1138 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
+        <v>27</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>13999</v>
+      </c>
+      <c r="F19" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" t="s">
+        <v>0</v>
+      </c>
+      <c r="K19" t="s">
+        <v>1</v>
+      </c>
+      <c r="L19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>28</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>33303</v>
+      </c>
+      <c r="F20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" t="s">
+        <v>3</v>
+      </c>
+      <c r="J20">
+        <f>AVERAGE(E1:E3)</f>
+        <v>17951</v>
+      </c>
+      <c r="K20">
+        <f>AVERAGE(E4:E6)</f>
+        <v>10849</v>
+      </c>
+      <c r="L20">
+        <f>AVERAGE(E7:E9)</f>
+        <v>13689</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>29</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>79574</v>
+      </c>
+      <c r="F21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" t="s">
+        <v>4</v>
+      </c>
+      <c r="J21">
+        <f>AVERAGE(E10:E12)</f>
+        <v>25999</v>
+      </c>
+      <c r="K21">
+        <f>AVERAGE(E13:E15)</f>
+        <v>19660.666666666668</v>
+      </c>
+      <c r="L21">
+        <f>AVERAGE(E16:E18)</f>
+        <v>20801.666666666668</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>30</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>15841</v>
+      </c>
+      <c r="F22" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" t="s">
+        <v>5</v>
+      </c>
+      <c r="J22">
+        <f>AVERAGE(E19:E21)</f>
+        <v>42292</v>
+      </c>
+      <c r="K22">
+        <f>AVERAGE(E22:E24)</f>
+        <v>29080</v>
+      </c>
+      <c r="L22">
+        <f>AVERAGE(E25:E27)</f>
+        <v>14057.666666666666</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>31</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>46759</v>
+      </c>
+      <c r="F23" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" t="s">
+        <v>6</v>
+      </c>
+      <c r="J23">
+        <f>AVERAGE(E28:E30)</f>
+        <v>135445.33333333334</v>
+      </c>
+      <c r="K23">
+        <f>AVERAGE(E31:E33)</f>
+        <v>53236.333333333336</v>
+      </c>
+      <c r="L23">
+        <f>AVERAGE(E34:E36)</f>
+        <v>36507.666666666664</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>32</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <v>24640</v>
+      </c>
+      <c r="F24" t="b">
+        <v>1</v>
+      </c>
+      <c r="I24" t="s">
+        <v>7</v>
+      </c>
+      <c r="J24">
+        <f>AVERAGE(E37:E39)</f>
+        <v>17131</v>
+      </c>
+      <c r="K24">
+        <f>AVERAGE(E40:E42)</f>
+        <v>31390.333333333332</v>
+      </c>
+      <c r="L24">
+        <f>AVERAGE(E43:E45)</f>
+        <v>15127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>33</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>13116</v>
+      </c>
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+      <c r="I25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J25">
+        <f>AVERAGE(E46:E48)</f>
+        <v>22500</v>
+      </c>
+      <c r="K25">
+        <f>AVERAGE(E49:E51)</f>
+        <v>32767</v>
+      </c>
+      <c r="L25">
+        <f>AVERAGE(E52:E54)</f>
+        <v>11544.333333333334</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>34</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>13745</v>
+      </c>
+      <c r="F26" t="b">
+        <v>1</v>
+      </c>
+      <c r="I26" t="s">
+        <v>14</v>
+      </c>
+      <c r="J26">
+        <f>AVERAGE(E55:E57)</f>
+        <v>29840</v>
+      </c>
+      <c r="K26">
+        <f>AVERAGE(E58:E60)</f>
+        <v>27985.666666666668</v>
+      </c>
+      <c r="L26">
+        <f>AVERAGE(E61:E63)</f>
+        <v>12321.666666666666</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>35</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27">
+        <v>15312</v>
+      </c>
+      <c r="F27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>45</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>122146</v>
+      </c>
+      <c r="F28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>46</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>267641</v>
+      </c>
+      <c r="F29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>47</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>16549</v>
+      </c>
+      <c r="F30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>48</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>28457</v>
+      </c>
+      <c r="F31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>49</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>34239</v>
+      </c>
+      <c r="F32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>50</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33">
+        <v>97013</v>
+      </c>
+      <c r="F33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>51</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>44998</v>
+      </c>
+      <c r="F34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>52</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>42102</v>
+      </c>
+      <c r="F35" t="b">
+        <v>1</v>
+      </c>
+      <c r="J35" t="s">
+        <v>3</v>
+      </c>
+      <c r="K35" t="s">
+        <v>4</v>
+      </c>
+      <c r="L35" t="s">
+        <v>5</v>
+      </c>
+      <c r="M35" t="s">
+        <v>6</v>
+      </c>
+      <c r="N35" t="s">
+        <v>7</v>
+      </c>
+      <c r="O35" t="s">
+        <v>10</v>
+      </c>
+      <c r="P35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>53</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36">
+        <v>22423</v>
+      </c>
+      <c r="F36" t="b">
+        <v>1</v>
+      </c>
+      <c r="I36" t="s">
+        <v>11</v>
+      </c>
+      <c r="J36">
+        <f>AVERAGE(E1,E4,E7)</f>
+        <v>11186</v>
+      </c>
+      <c r="K36">
+        <f>AVERAGE(E10,E13,E16)</f>
+        <v>26289.666666666668</v>
+      </c>
+      <c r="L36">
+        <f>AVERAGE(E19,E22,E25)</f>
+        <v>14318.666666666666</v>
+      </c>
+      <c r="M36">
+        <f>AVERAGE(E28,E31,E34)</f>
+        <v>65200.333333333336</v>
+      </c>
+      <c r="N36">
+        <f>AVERAGE(E37,E40,E43)</f>
+        <v>22839.666666666668</v>
+      </c>
+      <c r="O36">
+        <f>AVERAGE(E46,E49,E52)</f>
+        <v>13711</v>
+      </c>
+      <c r="P36">
+        <f>AVERAGE(E55,E58,E61)</f>
+        <v>13101.333333333334</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>54</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>24577</v>
+      </c>
+      <c r="F37" t="b">
+        <v>1</v>
+      </c>
+      <c r="I37" t="s">
+        <v>12</v>
+      </c>
+      <c r="J37">
+        <f t="shared" ref="J37:J38" si="0">AVERAGE(E2,E5,E8)</f>
+        <v>16817</v>
+      </c>
+      <c r="K37">
+        <f>AVERAGE(E11,E14,E17)</f>
+        <v>22193.666666666668</v>
+      </c>
+      <c r="L37">
+        <f>AVERAGE(E20,E23,E26)</f>
+        <v>31269</v>
+      </c>
+      <c r="M37">
+        <f>AVERAGE(E29,E32,E35)</f>
+        <v>114660.66666666667</v>
+      </c>
+      <c r="N37">
+        <f>AVERAGE(E38,E41,E44)</f>
+        <v>22751</v>
+      </c>
+      <c r="O37">
+        <f>AVERAGE(E47,E50,E53)</f>
+        <v>24976</v>
+      </c>
+      <c r="P37">
+        <f>AVERAGE(E56,E59,E62)</f>
+        <v>43402.333333333336</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>55</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>16271</v>
+      </c>
+      <c r="F38" t="b">
+        <v>1</v>
+      </c>
+      <c r="I38" t="s">
+        <v>13</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="0"/>
+        <v>14486</v>
+      </c>
+      <c r="K38">
+        <f>AVERAGE(E12,E15,E18)</f>
+        <v>17978</v>
+      </c>
+      <c r="L38">
+        <f>AVERAGE(E21,E24,E27)</f>
+        <v>39842</v>
+      </c>
+      <c r="M38">
+        <f>AVERAGE(E30,E33,E36)</f>
+        <v>45328.333333333336</v>
+      </c>
+      <c r="N38">
+        <f>AVERAGE(E39,E42,E45)</f>
+        <v>18057.666666666668</v>
+      </c>
+      <c r="O38">
+        <f>AVERAGE(E48,E51,E54)</f>
+        <v>28124.333333333332</v>
+      </c>
+      <c r="P38">
+        <f>AVERAGE(E57,E60,E63)</f>
+        <v>13643.666666666666</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>56</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39">
+        <v>10545</v>
+      </c>
+      <c r="F39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>57</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>31838</v>
+      </c>
+      <c r="F40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>58</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>39680</v>
+      </c>
+      <c r="F41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>59</v>
+      </c>
+      <c r="B42">
+        <v>4</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42">
+        <v>22653</v>
+      </c>
+      <c r="F42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>60</v>
+      </c>
+      <c r="B43">
+        <v>4</v>
+      </c>
+      <c r="C43" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>12104</v>
+      </c>
+      <c r="F43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>61</v>
+      </c>
+      <c r="B44">
+        <v>4</v>
+      </c>
+      <c r="C44" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>12302</v>
+      </c>
+      <c r="F44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>62</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="C45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="E45">
+        <v>20975</v>
+      </c>
+      <c r="F45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>36</v>
+      </c>
+      <c r="B46">
+        <v>5</v>
+      </c>
+      <c r="C46" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>18255</v>
+      </c>
+      <c r="F46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>37</v>
+      </c>
+      <c r="B47">
+        <v>5</v>
+      </c>
+      <c r="C47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>31967</v>
+      </c>
+      <c r="F47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>38</v>
+      </c>
+      <c r="B48">
+        <v>5</v>
+      </c>
+      <c r="C48" t="s">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48">
+        <v>17278</v>
+      </c>
+      <c r="F48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>39</v>
+      </c>
+      <c r="B49">
+        <v>5</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>8143</v>
+      </c>
+      <c r="F49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>40</v>
+      </c>
+      <c r="B50">
+        <v>5</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>31383</v>
+      </c>
+      <c r="F50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>41</v>
+      </c>
+      <c r="B51">
+        <v>5</v>
+      </c>
+      <c r="C51" t="s">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
+      </c>
+      <c r="E51">
+        <v>58775</v>
+      </c>
+      <c r="F51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>42</v>
+      </c>
+      <c r="B52">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>14735</v>
+      </c>
+      <c r="F52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>43</v>
+      </c>
+      <c r="B53">
+        <v>5</v>
+      </c>
+      <c r="C53" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>11578</v>
+      </c>
+      <c r="F53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>44</v>
+      </c>
+      <c r="B54">
+        <v>5</v>
+      </c>
+      <c r="C54" t="s">
+        <v>2</v>
+      </c>
+      <c r="D54">
+        <v>2</v>
+      </c>
+      <c r="E54">
+        <v>8320</v>
+      </c>
+      <c r="F54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55">
         <v>18</v>
       </c>
-      <c r="B19">
+      <c r="B55">
         <v>6</v>
       </c>
-      <c r="C19" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
+      <c r="C55" t="s">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
         <v>2988</v>
       </c>
-      <c r="F19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="F55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56">
         <v>19</v>
       </c>
-      <c r="B20">
+      <c r="B56">
         <v>6</v>
       </c>
-      <c r="C20" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
+      <c r="C56" t="s">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
         <v>65466</v>
       </c>
-      <c r="F20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="F56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B57">
         <v>6</v>
       </c>
-      <c r="C21" t="s">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>2</v>
-      </c>
-      <c r="E21">
+      <c r="C57" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57">
         <v>21066</v>
       </c>
-      <c r="F21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="F57" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58">
         <v>21</v>
       </c>
-      <c r="B22">
+      <c r="B58">
         <v>6</v>
       </c>
-      <c r="C22" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
+      <c r="C58" t="s">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
         <v>15216</v>
       </c>
-      <c r="F22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="F58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59">
         <v>22</v>
       </c>
-      <c r="B23">
+      <c r="B59">
         <v>6</v>
       </c>
-      <c r="C23" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23">
+      <c r="C59" t="s">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
         <v>57051</v>
       </c>
-      <c r="F23" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="F59" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60">
         <v>23</v>
       </c>
-      <c r="B24">
+      <c r="B60">
         <v>6</v>
       </c>
-      <c r="C24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24">
-        <v>2</v>
-      </c>
-      <c r="E24">
+      <c r="C60" t="s">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>2</v>
+      </c>
+      <c r="E60">
         <v>11690</v>
       </c>
-      <c r="F24" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="F60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61">
         <v>24</v>
       </c>
-      <c r="B25">
+      <c r="B61">
         <v>6</v>
       </c>
-      <c r="C25" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
+      <c r="C61" t="s">
+        <v>2</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
         <v>21100</v>
       </c>
-      <c r="F25" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="F61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62">
         <v>25</v>
       </c>
-      <c r="B26">
+      <c r="B62">
         <v>6</v>
       </c>
-      <c r="C26" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26">
+      <c r="C62" t="s">
+        <v>2</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
         <v>7690</v>
       </c>
-      <c r="F26" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="F62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63">
         <v>26</v>
       </c>
-      <c r="B27">
+      <c r="B63">
         <v>6</v>
       </c>
-      <c r="C27" t="s">
-        <v>2</v>
-      </c>
-      <c r="D27">
-        <v>2</v>
-      </c>
-      <c r="E27">
+      <c r="C63" t="s">
+        <v>2</v>
+      </c>
+      <c r="D63">
+        <v>2</v>
+      </c>
+      <c r="E63">
         <v>8175</v>
       </c>
-      <c r="F27" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28">
-        <v>2</v>
-      </c>
-      <c r="C28" t="s">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>13999</v>
-      </c>
-      <c r="F28" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29">
-        <v>2</v>
-      </c>
-      <c r="C29" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29">
-        <v>33303</v>
-      </c>
-      <c r="F29" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30">
-        <v>2</v>
-      </c>
-      <c r="C30" t="s">
-        <v>0</v>
-      </c>
-      <c r="D30">
-        <v>2</v>
-      </c>
-      <c r="E30">
-        <v>79574</v>
-      </c>
-      <c r="F30" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31">
-        <v>2</v>
-      </c>
-      <c r="C31" t="s">
-        <v>1</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>15841</v>
-      </c>
-      <c r="F31" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32">
-        <v>2</v>
-      </c>
-      <c r="C32" t="s">
-        <v>1</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32">
-        <v>46759</v>
-      </c>
-      <c r="F32" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33">
-        <v>2</v>
-      </c>
-      <c r="C33" t="s">
-        <v>1</v>
-      </c>
-      <c r="D33">
-        <v>2</v>
-      </c>
-      <c r="E33">
-        <v>24640</v>
-      </c>
-      <c r="F33" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34">
-        <v>2</v>
-      </c>
-      <c r="C34" t="s">
-        <v>2</v>
-      </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34">
-        <v>13116</v>
-      </c>
-      <c r="F34" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35">
-        <v>2</v>
-      </c>
-      <c r="C35" t="s">
-        <v>2</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35">
-        <v>13745</v>
-      </c>
-      <c r="F35" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="B36">
-        <v>2</v>
-      </c>
-      <c r="C36" t="s">
-        <v>2</v>
-      </c>
-      <c r="D36">
-        <v>2</v>
-      </c>
-      <c r="E36">
-        <v>15312</v>
-      </c>
-      <c r="F36" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="B37">
-        <v>5</v>
-      </c>
-      <c r="C37" t="s">
-        <v>0</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>18255</v>
-      </c>
-      <c r="F37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>37</v>
-      </c>
-      <c r="B38">
-        <v>5</v>
-      </c>
-      <c r="C38" t="s">
-        <v>0</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38">
-        <v>31967</v>
-      </c>
-      <c r="F38" t="b">
-        <v>1</v>
-      </c>
-      <c r="J38" t="s">
-        <v>0</v>
-      </c>
-      <c r="K38" t="s">
-        <v>1</v>
-      </c>
-      <c r="L38" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="B39">
-        <v>5</v>
-      </c>
-      <c r="C39" t="s">
-        <v>0</v>
-      </c>
-      <c r="D39">
-        <v>2</v>
-      </c>
-      <c r="E39">
-        <v>17278</v>
-      </c>
-      <c r="F39" t="b">
-        <v>1</v>
-      </c>
-      <c r="I39" t="s">
-        <v>10</v>
-      </c>
-      <c r="J39">
-        <v>9817</v>
-      </c>
-      <c r="K39">
-        <v>9759</v>
-      </c>
-      <c r="L39">
-        <v>13982</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="B40">
-        <v>5</v>
-      </c>
-      <c r="C40" t="s">
-        <v>1</v>
-      </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="E40">
-        <v>8143</v>
-      </c>
-      <c r="F40" t="b">
-        <v>1</v>
-      </c>
-      <c r="I40" t="s">
-        <v>10</v>
-      </c>
-      <c r="J40">
-        <v>26790</v>
-      </c>
-      <c r="K40">
-        <v>11558</v>
-      </c>
-      <c r="L40">
-        <v>12103</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>40</v>
-      </c>
-      <c r="B41">
-        <v>5</v>
-      </c>
-      <c r="C41" t="s">
-        <v>1</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41">
-        <v>31383</v>
-      </c>
-      <c r="F41" t="b">
-        <v>1</v>
-      </c>
-      <c r="I41" t="s">
-        <v>10</v>
-      </c>
-      <c r="J41">
-        <v>17246</v>
-      </c>
-      <c r="K41">
-        <v>11230</v>
-      </c>
-      <c r="L41">
-        <v>14982</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>41</v>
-      </c>
-      <c r="B42">
-        <v>5</v>
-      </c>
-      <c r="C42" t="s">
-        <v>1</v>
-      </c>
-      <c r="D42">
-        <v>2</v>
-      </c>
-      <c r="E42">
-        <v>58775</v>
-      </c>
-      <c r="F42" t="b">
-        <v>1</v>
-      </c>
-      <c r="I42" t="s">
-        <v>4</v>
-      </c>
-      <c r="J42">
-        <v>35865</v>
-      </c>
-      <c r="K42">
-        <v>15042</v>
-      </c>
-      <c r="L42">
-        <v>27962</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>42</v>
-      </c>
-      <c r="B43">
-        <v>5</v>
-      </c>
-      <c r="C43" t="s">
-        <v>2</v>
-      </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
-      <c r="E43">
-        <v>14735</v>
-      </c>
-      <c r="F43" t="b">
-        <v>1</v>
-      </c>
-      <c r="I43" t="s">
-        <v>4</v>
-      </c>
-      <c r="J43">
-        <v>24914</v>
-      </c>
-      <c r="K43">
-        <v>22034</v>
-      </c>
-      <c r="L43">
-        <v>19633</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>43</v>
-      </c>
-      <c r="B44">
-        <v>5</v>
-      </c>
-      <c r="C44" t="s">
-        <v>2</v>
-      </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="E44">
-        <v>11578</v>
-      </c>
-      <c r="F44" t="b">
-        <v>1</v>
-      </c>
-      <c r="I44" t="s">
-        <v>4</v>
-      </c>
-      <c r="J44">
-        <v>17218</v>
-      </c>
-      <c r="K44">
-        <v>21906</v>
-      </c>
-      <c r="L44">
-        <v>14810</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>44</v>
-      </c>
-      <c r="B45">
-        <v>5</v>
-      </c>
-      <c r="C45" t="s">
-        <v>2</v>
-      </c>
-      <c r="D45">
-        <v>2</v>
-      </c>
-      <c r="E45">
-        <v>8320</v>
-      </c>
-      <c r="F45" t="b">
-        <v>1</v>
-      </c>
-      <c r="I45" t="s">
-        <v>9</v>
-      </c>
-      <c r="J45">
-        <v>2988</v>
-      </c>
-      <c r="K45">
-        <v>15216</v>
-      </c>
-      <c r="L45">
-        <v>21100</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>45</v>
-      </c>
-      <c r="B46">
-        <v>3</v>
-      </c>
-      <c r="C46" t="s">
-        <v>0</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46">
-        <v>122146</v>
-      </c>
-      <c r="F46" t="b">
-        <v>1</v>
-      </c>
-      <c r="I46" t="s">
-        <v>9</v>
-      </c>
-      <c r="J46">
-        <v>65466</v>
-      </c>
-      <c r="K46">
-        <v>57051</v>
-      </c>
-      <c r="L46">
-        <v>7690</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>46</v>
-      </c>
-      <c r="B47">
-        <v>3</v>
-      </c>
-      <c r="C47" t="s">
-        <v>0</v>
-      </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-      <c r="E47">
-        <v>267641</v>
-      </c>
-      <c r="F47" t="b">
-        <v>0</v>
-      </c>
-      <c r="I47" t="s">
-        <v>9</v>
-      </c>
-      <c r="J47">
-        <v>21066</v>
-      </c>
-      <c r="K47">
-        <v>11690</v>
-      </c>
-      <c r="L47">
-        <v>8175</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>47</v>
-      </c>
-      <c r="B48">
-        <v>3</v>
-      </c>
-      <c r="C48" t="s">
-        <v>0</v>
-      </c>
-      <c r="D48">
-        <v>2</v>
-      </c>
-      <c r="E48">
-        <v>16549</v>
-      </c>
-      <c r="F48" t="b">
-        <v>1</v>
-      </c>
-      <c r="I48" t="s">
-        <v>5</v>
-      </c>
-      <c r="J48">
-        <v>13999</v>
-      </c>
-      <c r="K48">
-        <v>15841</v>
-      </c>
-      <c r="L48">
-        <v>13116</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>48</v>
-      </c>
-      <c r="B49">
-        <v>3</v>
-      </c>
-      <c r="C49" t="s">
-        <v>1</v>
-      </c>
-      <c r="D49">
-        <v>0</v>
-      </c>
-      <c r="E49">
-        <v>28457</v>
-      </c>
-      <c r="F49" t="b">
-        <v>1</v>
-      </c>
-      <c r="I49" t="s">
-        <v>5</v>
-      </c>
-      <c r="J49">
-        <v>33303</v>
-      </c>
-      <c r="K49">
-        <v>46759</v>
-      </c>
-      <c r="L49">
-        <v>13745</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>49</v>
-      </c>
-      <c r="B50">
-        <v>3</v>
-      </c>
-      <c r="C50" t="s">
-        <v>1</v>
-      </c>
-      <c r="D50">
-        <v>1</v>
-      </c>
-      <c r="E50">
-        <v>34239</v>
-      </c>
-      <c r="F50" t="b">
-        <v>1</v>
-      </c>
-      <c r="I50" t="s">
-        <v>5</v>
-      </c>
-      <c r="J50">
-        <v>79574</v>
-      </c>
-      <c r="K50">
-        <v>24640</v>
-      </c>
-      <c r="L50">
-        <v>15312</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>50</v>
-      </c>
-      <c r="B51">
-        <v>3</v>
-      </c>
-      <c r="C51" t="s">
-        <v>1</v>
-      </c>
-      <c r="D51">
-        <v>2</v>
-      </c>
-      <c r="E51">
-        <v>97013</v>
-      </c>
-      <c r="F51" t="b">
-        <v>1</v>
-      </c>
-      <c r="I51" t="s">
-        <v>11</v>
-      </c>
-      <c r="J51">
-        <v>18255</v>
-      </c>
-      <c r="K51">
-        <v>8143</v>
-      </c>
-      <c r="L51">
-        <v>14735</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>51</v>
-      </c>
-      <c r="B52">
-        <v>3</v>
-      </c>
-      <c r="C52" t="s">
-        <v>2</v>
-      </c>
-      <c r="D52">
-        <v>0</v>
-      </c>
-      <c r="E52">
-        <v>44998</v>
-      </c>
-      <c r="F52" t="b">
-        <v>1</v>
-      </c>
-      <c r="I52" t="s">
-        <v>11</v>
-      </c>
-      <c r="J52">
-        <v>31967</v>
-      </c>
-      <c r="K52">
-        <v>31383</v>
-      </c>
-      <c r="L52">
-        <v>11578</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>52</v>
-      </c>
-      <c r="B53">
-        <v>3</v>
-      </c>
-      <c r="C53" t="s">
-        <v>2</v>
-      </c>
-      <c r="D53">
-        <v>1</v>
-      </c>
-      <c r="E53">
-        <v>42102</v>
-      </c>
-      <c r="F53" t="b">
-        <v>1</v>
-      </c>
-      <c r="I53" t="s">
-        <v>11</v>
-      </c>
-      <c r="J53">
-        <v>17278</v>
-      </c>
-      <c r="K53">
-        <v>58775</v>
-      </c>
-      <c r="L53">
-        <v>8320</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>53</v>
-      </c>
-      <c r="B54">
-        <v>3</v>
-      </c>
-      <c r="C54" t="s">
-        <v>2</v>
-      </c>
-      <c r="D54">
-        <v>2</v>
-      </c>
-      <c r="E54">
-        <v>22423</v>
-      </c>
-      <c r="F54" t="b">
-        <v>1</v>
-      </c>
-      <c r="I54" t="s">
-        <v>6</v>
-      </c>
-      <c r="J54">
-        <v>122146</v>
-      </c>
-      <c r="K54">
-        <v>28457</v>
-      </c>
-      <c r="L54">
-        <v>44998</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>54</v>
-      </c>
-      <c r="B55">
-        <v>4</v>
-      </c>
-      <c r="C55" t="s">
-        <v>0</v>
-      </c>
-      <c r="D55">
-        <v>0</v>
-      </c>
-      <c r="E55">
-        <v>24577</v>
-      </c>
-      <c r="F55" t="b">
-        <v>1</v>
-      </c>
-      <c r="I55" t="s">
-        <v>6</v>
-      </c>
-      <c r="J55">
-        <v>267641</v>
-      </c>
-      <c r="K55">
-        <v>34239</v>
-      </c>
-      <c r="L55">
-        <v>42102</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>55</v>
-      </c>
-      <c r="B56">
-        <v>4</v>
-      </c>
-      <c r="C56" t="s">
-        <v>0</v>
-      </c>
-      <c r="D56">
-        <v>1</v>
-      </c>
-      <c r="E56">
-        <v>16271</v>
-      </c>
-      <c r="F56" t="b">
-        <v>1</v>
-      </c>
-      <c r="I56" t="s">
-        <v>6</v>
-      </c>
-      <c r="J56">
-        <v>16549</v>
-      </c>
-      <c r="K56">
-        <v>97013</v>
-      </c>
-      <c r="L56">
-        <v>22423</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>56</v>
-      </c>
-      <c r="B57">
-        <v>4</v>
-      </c>
-      <c r="C57" t="s">
-        <v>0</v>
-      </c>
-      <c r="D57">
-        <v>2</v>
-      </c>
-      <c r="E57">
-        <v>10545</v>
-      </c>
-      <c r="F57" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>57</v>
-      </c>
-      <c r="B58">
-        <v>4</v>
-      </c>
-      <c r="C58" t="s">
-        <v>1</v>
-      </c>
-      <c r="D58">
-        <v>0</v>
-      </c>
-      <c r="E58">
-        <v>31838</v>
-      </c>
-      <c r="F58" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>58</v>
-      </c>
-      <c r="B59">
-        <v>4</v>
-      </c>
-      <c r="C59" t="s">
-        <v>1</v>
-      </c>
-      <c r="D59">
-        <v>1</v>
-      </c>
-      <c r="E59">
-        <v>39680</v>
-      </c>
-      <c r="F59" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>59</v>
-      </c>
-      <c r="B60">
-        <v>4</v>
-      </c>
-      <c r="C60" t="s">
-        <v>1</v>
-      </c>
-      <c r="D60">
-        <v>2</v>
-      </c>
-      <c r="E60">
-        <v>22653</v>
-      </c>
-      <c r="F60" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>60</v>
-      </c>
-      <c r="B61">
-        <v>4</v>
-      </c>
-      <c r="C61" t="s">
-        <v>2</v>
-      </c>
-      <c r="D61">
-        <v>0</v>
-      </c>
-      <c r="E61">
-        <v>12104</v>
-      </c>
-      <c r="F61" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>61</v>
-      </c>
-      <c r="B62">
-        <v>4</v>
-      </c>
-      <c r="C62" t="s">
-        <v>2</v>
-      </c>
-      <c r="D62">
-        <v>1</v>
-      </c>
-      <c r="E62">
-        <v>12302</v>
-      </c>
-      <c r="F62" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>62</v>
-      </c>
-      <c r="B63">
-        <v>4</v>
-      </c>
-      <c r="C63" t="s">
-        <v>2</v>
-      </c>
-      <c r="D63">
-        <v>2</v>
-      </c>
-      <c r="E63">
-        <v>20975</v>
-      </c>
       <c r="F63" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A1:F63">
+    <sortCondition ref="B1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -3081,7 +3326,7 @@
     </row>
     <row r="17" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G17">
         <v>9817</v>
@@ -3095,7 +3340,7 @@
     </row>
     <row r="18" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G18">
         <v>26790</v>
@@ -3109,7 +3354,7 @@
     </row>
     <row r="19" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G19">
         <v>17246</v>
@@ -3165,7 +3410,7 @@
     </row>
     <row r="23" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G23">
         <v>2988</v>
@@ -3179,7 +3424,7 @@
     </row>
     <row r="24" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G24">
         <v>65466</v>
@@ -3193,7 +3438,7 @@
     </row>
     <row r="25" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G25">
         <v>21066</v>
@@ -3249,7 +3494,7 @@
     </row>
     <row r="29" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G29">
         <v>18255</v>
@@ -3263,7 +3508,7 @@
     </row>
     <row r="30" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G30">
         <v>31967</v>
@@ -3277,7 +3522,7 @@
     </row>
     <row r="31" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G31">
         <v>17278</v>

</xml_diff>